<commit_message>
First delivery of compliancy test stylesheets.
</commit_message>
<xml_diff>
--- a/src/main/resources/cfg/ComplyCompiler/templates/Testberichten sjabloon leeg.xlsx
+++ b/src/main/resources/cfg/ComplyCompiler/templates/Testberichten sjabloon leeg.xlsx
@@ -23,21 +23,7 @@
     <author>Frank Samwel</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Compliancy testberichten sjabloon gegenereerd door imvertor</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
+	</commentList>
 </comments>
 </file>
 
@@ -47,21 +33,7 @@
     <author>Frank Samwel</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Compliancy testberichten sjabloon gegenereerd door imvertor</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
+	</commentList>
 </comments>
 </file>
 
@@ -285,7 +257,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <!-- s="1" -->
@@ -331,6 +303,10 @@
       <!-- s="18" -->
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
+    <!-- s="19": choice element met link naar gegevensgroep  -->
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <!-- s="20": laatste choice element met link naar gegevensgroep  -->
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -447,10 +423,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:K3">
-    <cfRule type="expression" dxfId="1" priority="9998" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="7998" stopIfTrue="1">
       <formula>OR($C3="",MID($C3,1,1)="0")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="9999" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="7999" stopIfTrue="1">
       <formula>OR($B3="CHOICE",$B3="SEQUENCE")</formula>
     </cfRule>
     <cfRule type="containsBlanks" dxfId="2" priority="10000">
@@ -518,10 +494,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:K3">
-    <cfRule type="expression" dxfId="1" priority="9998" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="7998" stopIfTrue="1">
       <formula>OR($C3="",MID($C3,1,1)="0")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="9999" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="7999" stopIfTrue="1">
       <formula>OR($B3="CHOICE",$B3="SEQUENCE")</formula>
     </cfRule>
     <cfRule type="containsBlanks" dxfId="2" priority="10000">

</xml_diff>